<commit_message>
Reorganized and knitted scripts
</commit_message>
<xml_diff>
--- a/data/processed/OSM_all_config_covariates_correlation.xlsx
+++ b/data/processed/OSM_all_config_covariates_correlation.xlsx
@@ -7,26 +7,28 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="250m" sheetId="1" r:id="rId1"/>
-    <sheet name="500m" sheetId="2" r:id="rId2"/>
-    <sheet name="750m" sheetId="3" r:id="rId3"/>
-    <sheet name="1000m" sheetId="4" r:id="rId4"/>
-    <sheet name="1250m" sheetId="5" r:id="rId5"/>
-    <sheet name="1500m" sheetId="6" r:id="rId6"/>
-    <sheet name="1750m" sheetId="7" r:id="rId7"/>
-    <sheet name="2000m" sheetId="8" r:id="rId8"/>
-    <sheet name="2250m" sheetId="9" r:id="rId9"/>
-    <sheet name="2500m" sheetId="10" r:id="rId10"/>
-    <sheet name="2750m" sheetId="11" r:id="rId11"/>
-    <sheet name="3000m" sheetId="12" r:id="rId12"/>
-    <sheet name="3250m" sheetId="13" r:id="rId13"/>
-    <sheet name="3500m" sheetId="14" r:id="rId14"/>
-    <sheet name="3750m" sheetId="15" r:id="rId15"/>
-    <sheet name="4000m" sheetId="16" r:id="rId16"/>
-    <sheet name="4250m" sheetId="17" r:id="rId17"/>
-    <sheet name="4500m" sheetId="18" r:id="rId18"/>
-    <sheet name="4750m" sheetId="19" r:id="rId19"/>
-    <sheet name="5000m" sheetId="20" r:id="rId20"/>
+    <sheet name="50m" sheetId="1" r:id="rId1"/>
+    <sheet name="100m" sheetId="2" r:id="rId2"/>
+    <sheet name="250m" sheetId="3" r:id="rId3"/>
+    <sheet name="500m" sheetId="4" r:id="rId4"/>
+    <sheet name="750m" sheetId="5" r:id="rId5"/>
+    <sheet name="1000m" sheetId="6" r:id="rId6"/>
+    <sheet name="1250m" sheetId="7" r:id="rId7"/>
+    <sheet name="1500m" sheetId="8" r:id="rId8"/>
+    <sheet name="1750m" sheetId="9" r:id="rId9"/>
+    <sheet name="2000m" sheetId="10" r:id="rId10"/>
+    <sheet name="2250m" sheetId="11" r:id="rId11"/>
+    <sheet name="2500m" sheetId="12" r:id="rId12"/>
+    <sheet name="2750m" sheetId="13" r:id="rId13"/>
+    <sheet name="3000m" sheetId="14" r:id="rId14"/>
+    <sheet name="3250m" sheetId="15" r:id="rId15"/>
+    <sheet name="3500m" sheetId="16" r:id="rId16"/>
+    <sheet name="3750m" sheetId="17" r:id="rId17"/>
+    <sheet name="4000m" sheetId="18" r:id="rId18"/>
+    <sheet name="4250m" sheetId="19" r:id="rId19"/>
+    <sheet name="4500m" sheetId="20" r:id="rId20"/>
+    <sheet name="4750m" sheetId="21" r:id="rId21"/>
+    <sheet name="5000m" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -2344,6 +2346,310 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_tca</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_ed</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_cai_mn</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_tca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_siei</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_shei</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_np</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_mesh</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_ed</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_contag</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>landscape_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>landscape_contag</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>landscape_ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>landscape_mesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>landscape_np</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>landscape_shei</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>landscape_siei</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>landscape_tca</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>nonanthro_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>nonanthro_ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>nonanthro_tca</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_tca</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_ed</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nonanthro_cai_mn</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_tca</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_siei</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_shei</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_np</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_mesh</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_ed</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_contag</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>landscape_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>landscape_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>landscape_contag</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>landscape_ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>landscape_mesh</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>landscape_np</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>landscape_shei</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>landscape_siei</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>landscape_tca</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>nonanthro_cai_mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>nonanthro_ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>nonanthro_tca</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L12"/>

</xml_diff>